<commit_message>
Manage Interviewers flow -Done
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/INTERVIEW_CANCELLATION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/INTERVIEW_CANCELLATION_HISTORY_DATA.xlsx
@@ -1386,39 +1386,85 @@
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="6">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>2021-06-11</t>
         </is>
       </c>
       <c r="B10" s="10" t="n">
-        <v>44358.66002977454</v>
-      </c>
-      <c r="C10" t="inlineStr">
+        <v>44358.66002978009</v>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
         <is>
           <t>pavan_demo_145</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="5" t="n">
         <v>119</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="5" t="n">
         <v>117</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="5" t="n">
         <v>2.95</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
-      <c r="B11" s="8" t="n"/>
-      <c r="D11" s="9" t="n"/>
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>2021-06-16</t>
+        </is>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>44363.69445333333</v>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>live_145_hotfix</t>
+        </is>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>119</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>4.24</v>
+      </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
-      <c r="B12" s="8" t="n"/>
-      <c r="D12" s="9" t="n"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-06-16</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>44363.81532318905</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>live_145_hf2</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>119</v>
+      </c>
+      <c r="E12" t="n">
+        <v>117</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2.87</v>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
       <c r="B13" s="8" t="n"/>

</xml_diff>